<commit_message>
the sixth time commit
</commit_message>
<xml_diff>
--- a/excel_testcase/testdata.xlsx
+++ b/excel_testcase/testdata.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\UiAutomation\WuLiuUiAutomation\excel_testcase\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="7950" windowWidth="20385" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Suite" r:id="rId1" sheetId="1"/>
-    <sheet name="HuoZhuSteps" r:id="rId2" sheetId="4"/>
-    <sheet name="GouShuiNiStep" r:id="rId3" sheetId="2"/>
-    <sheet name="KeyWords" r:id="rId4" sheetId="3"/>
-    <sheet name="Sheet1" r:id="rId5" sheetId="5"/>
+    <sheet name="Suite" sheetId="1" r:id="rId1"/>
+    <sheet name="HuoZhuSteps" sheetId="4" r:id="rId2"/>
+    <sheet name="GouShuiNiStep" sheetId="2" r:id="rId3"/>
+    <sheet name="KeyWords" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -30,7 +30,7 @@
     <author>作者</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A1" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -54,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="B1" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -78,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="C1" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -102,7 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="D1" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -126,7 +126,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="E1" shapeId="0">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -150,7 +150,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="F1" shapeId="0">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -174,7 +174,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="G1" shapeId="0">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -198,7 +198,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="H1" shapeId="0">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -222,7 +222,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="M1" shapeId="0">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -246,7 +246,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="N1" shapeId="0">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -270,7 +270,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="O1" shapeId="0">
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -294,7 +294,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="D2" shapeId="0">
+    <comment ref="D2" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -318,7 +318,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="G2" shapeId="0">
+    <comment ref="G2" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -344,7 +344,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="D3" shapeId="0">
+    <comment ref="D3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -368,7 +368,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="I5" shapeId="0">
+    <comment ref="I5" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -392,7 +392,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="I6" shapeId="0">
+    <comment ref="I6" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -416,7 +416,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="I27" shapeId="0">
+    <comment ref="I27" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -440,7 +440,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="2" ref="J27" shapeId="0">
+    <comment ref="J27" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -464,7 +464,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="G37" shapeId="0">
+    <comment ref="G37" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -488,7 +488,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="G40" shapeId="0">
+    <comment ref="G40" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -512,7 +512,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="K40" shapeId="0">
+    <comment ref="K40" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -536,7 +536,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="J42" shapeId="0">
+    <comment ref="J42" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -560,7 +560,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="I44" shapeId="0">
+    <comment ref="I44" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -584,7 +584,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="G59" shapeId="0">
+    <comment ref="G59" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -608,7 +608,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="I59" shapeId="0">
+    <comment ref="I59" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -632,7 +632,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="K59" shapeId="0">
+    <comment ref="K59" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -656,7 +656,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="G60" shapeId="0">
+    <comment ref="G60" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -680,7 +680,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="I60" shapeId="0">
+    <comment ref="I60" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -704,7 +704,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="G64" shapeId="0">
+    <comment ref="G64" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -728,7 +728,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="I64" shapeId="0">
+    <comment ref="I64" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -752,7 +752,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="I71" shapeId="0">
+    <comment ref="I71" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -778,7 +778,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="I78" shapeId="0">
+    <comment ref="I78" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -802,7 +802,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="I87" shapeId="0">
+    <comment ref="I87" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -826,7 +826,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="I91" shapeId="0">
+    <comment ref="I91" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -850,7 +850,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="I93" shapeId="0">
+    <comment ref="I93" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -874,7 +874,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="G98" shapeId="0">
+    <comment ref="G98" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -898,7 +898,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="I98" shapeId="0">
+    <comment ref="I98" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -922,7 +922,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="G99" shapeId="0">
+    <comment ref="G99" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -946,7 +946,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="I99" shapeId="0">
+    <comment ref="I99" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -970,7 +970,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="I102" shapeId="0">
+    <comment ref="I102" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -994,7 +994,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="G114" shapeId="0">
+    <comment ref="G114" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1018,7 +1018,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="I114" shapeId="0">
+    <comment ref="I114" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1042,7 +1042,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="K114" shapeId="0">
+    <comment ref="K114" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1066,7 +1066,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="G124" shapeId="0">
+    <comment ref="G125" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1090,7 +1090,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="I124" shapeId="0">
+    <comment ref="I125" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1114,7 +1114,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="K124" shapeId="0">
+    <comment ref="K125" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1138,7 +1138,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="I131" shapeId="0">
+    <comment ref="I132" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1176,7 +1176,7 @@
     <author>joy</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A1" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1200,7 +1200,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="B1" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1224,7 +1224,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="C1" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1248,7 +1248,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="D1" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1272,7 +1272,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="E1" shapeId="0">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1296,7 +1296,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="F1" shapeId="0">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1320,7 +1320,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="G1" shapeId="0">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1344,7 +1344,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="H1" shapeId="0">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1368,7 +1368,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="M1" shapeId="0">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1392,7 +1392,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="N1" shapeId="0">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1416,7 +1416,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="O1" shapeId="0">
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1440,7 +1440,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="I2" shapeId="0">
+    <comment ref="I2" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1464,7 +1464,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="J2" shapeId="0">
+    <comment ref="J2" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1488,7 +1488,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="2" ref="I14" shapeId="0">
+    <comment ref="I14" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1512,7 +1512,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="2" ref="I19" shapeId="0">
+    <comment ref="I19" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1536,7 +1536,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="J19" shapeId="0">
+    <comment ref="J19" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1560,7 +1560,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="2" ref="G30" shapeId="0">
+    <comment ref="G30" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1584,7 +1584,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="2" ref="G33" shapeId="0">
+    <comment ref="G33" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1608,7 +1608,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="2" ref="K33" shapeId="0">
+    <comment ref="K33" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1632,7 +1632,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="2" ref="K35" shapeId="0">
+    <comment ref="K35" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1656,7 +1656,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="2" ref="I37" shapeId="0">
+    <comment ref="I37" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1680,7 +1680,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="2" ref="G48" shapeId="0">
+    <comment ref="G48" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1704,7 +1704,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="2" ref="I48" shapeId="0">
+    <comment ref="I48" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1728,7 +1728,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="2" ref="K48" shapeId="0">
+    <comment ref="K48" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1752,7 +1752,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="2" ref="G50" shapeId="0">
+    <comment ref="G50" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1776,7 +1776,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="2" ref="I50" shapeId="0">
+    <comment ref="I50" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1800,7 +1800,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="2" ref="I56" shapeId="0">
+    <comment ref="I56" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1824,7 +1824,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="2" ref="I64" shapeId="0">
+    <comment ref="I64" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1848,7 +1848,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="2" ref="I65" shapeId="0">
+    <comment ref="I65" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1872,7 +1872,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="2" ref="I70" shapeId="0">
+    <comment ref="I70" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1896,7 +1896,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="2" ref="I72" shapeId="0">
+    <comment ref="I72" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1920,7 +1920,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="2" ref="I74" shapeId="0">
+    <comment ref="I74" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1944,7 +1944,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="2" ref="I76" shapeId="0">
+    <comment ref="I76" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1968,7 +1968,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="2" ref="I81" shapeId="0">
+    <comment ref="I81" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1992,7 +1992,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="2" ref="G85" shapeId="0">
+    <comment ref="G85" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2016,7 +2016,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="2" ref="I85" shapeId="0">
+    <comment ref="I85" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2040,7 +2040,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="2" ref="G87" shapeId="0">
+    <comment ref="G87" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2064,7 +2064,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="2" ref="I87" shapeId="0">
+    <comment ref="I87" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2088,7 +2088,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="2" ref="I90" shapeId="0">
+    <comment ref="I90" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2112,7 +2112,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="2" ref="I99" shapeId="0">
+    <comment ref="I99" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2136,7 +2136,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="I102" shapeId="0">
+    <comment ref="I102" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2160,7 +2160,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="1" ref="J102" shapeId="0">
+    <comment ref="J102" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2194,7 +2194,7 @@
     <author>joy</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="B26" shapeId="0">
+    <comment ref="B26" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2228,7 +2228,7 @@
     <author>joy</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="I2" shapeId="0">
+    <comment ref="I2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2252,7 +2252,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="G10" shapeId="0">
+    <comment ref="G10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2276,7 +2276,7 @@
         </r>
       </text>
     </comment>
-    <comment authorId="0" ref="I10" shapeId="0">
+    <comment ref="I10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2305,7 +2305,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2599" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2575" uniqueCount="543">
   <si>
     <t>测试用例</t>
   </si>
@@ -4958,18 +4958,21 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>测试用例执行成功</t>
-  </si>
-  <si>
     <t>测试用例执行失败</t>
+  </si>
+  <si>
+    <t>浙AS1237</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>test143</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5052,14 +5055,6 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -5079,91 +5074,88 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+  <cellXfs count="33">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" quotePrefix="1" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="8" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="8" numFmtId="0" quotePrefix="1" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="0" name="常规" xfId="0"/>
-    <cellStyle builtinId="8" name="超链接" xfId="1"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -5180,10 +5172,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -5218,7 +5210,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5253,7 +5245,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5341,7 +5333,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -5350,13 +5342,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -5366,7 +5358,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -5375,7 +5367,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -5384,7 +5376,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -5394,12 +5386,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -5430,7 +5422,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -5449,7 +5441,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -5461,8 +5453,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
@@ -5470,11 +5462,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="36.75" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="23.625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="17.625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="23.625" collapsed="true"/>
+    <col min="1" max="1" width="14.875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36.75" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -5522,48 +5514,48 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="D2:D3" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3">
       <formula1>"YES,NO"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.69930555555555596" right="0.69930555555555596" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
-  <dimension ref="A1:P143"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="B55" sqref="B55:B143"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I121" sqref="I121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="8.125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="5.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="5.875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="6.125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="14.75" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="10.625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="12" width="18.625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="16.875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="12.125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="40.75" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="19.5" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="18.5" collapsed="true"/>
+    <col min="1" max="1" width="10.5" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="5" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="5.875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="6.125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.75" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18.625" style="12" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="40.75" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="19.5" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="18.5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="27" r="1" spans="1:15">
+    <row r="1" spans="1:15" ht="27">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -7077,7 +7069,7 @@
         <v>478</v>
       </c>
     </row>
-    <row ht="27" r="40" spans="1:15">
+    <row r="40" spans="1:15" ht="27">
       <c r="A40" s="14" t="s">
         <v>530</v>
       </c>
@@ -7157,7 +7149,7 @@
         <v>478</v>
       </c>
     </row>
-    <row ht="27" r="42" spans="1:15">
+    <row r="42" spans="1:15" ht="27">
       <c r="A42" s="14" t="s">
         <v>530</v>
       </c>
@@ -7806,7 +7798,7 @@
         <v>478</v>
       </c>
     </row>
-    <row ht="27" r="59" spans="1:15">
+    <row r="59" spans="1:15" ht="27">
       <c r="A59" s="14" t="s">
         <v>530</v>
       </c>
@@ -8282,7 +8274,7 @@
       <c r="E71" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="F71" s="33" t="s">
+      <c r="F71" s="30" t="s">
         <v>529</v>
       </c>
       <c r="G71" s="15" t="s">
@@ -8916,7 +8908,9 @@
         <v>252</v>
       </c>
       <c r="N87" s="5"/>
-      <c r="O87" s="5"/>
+      <c r="O87" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="88" spans="1:15">
       <c r="A88" s="14" t="s">
@@ -8952,7 +8946,9 @@
         <v>258</v>
       </c>
       <c r="N88" s="5"/>
-      <c r="O88" s="5"/>
+      <c r="O88" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="89" spans="1:15">
       <c r="A89" s="14" t="s">
@@ -8981,7 +8977,7 @@
         <v>buttonClick</v>
       </c>
       <c r="I89" s="17" t="s">
-        <v>261</v>
+        <v>541</v>
       </c>
       <c r="J89" s="5"/>
       <c r="K89" s="5"/>
@@ -8990,7 +8986,9 @@
         <v>252</v>
       </c>
       <c r="N89" s="5"/>
-      <c r="O89" s="5"/>
+      <c r="O89" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="90" spans="1:15">
       <c r="A90" s="14" t="s">
@@ -9026,7 +9024,9 @@
         <v>264</v>
       </c>
       <c r="N90" s="5"/>
-      <c r="O90" s="5"/>
+      <c r="O90" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="91" spans="1:15">
       <c r="A91" s="14" t="s">
@@ -9062,7 +9062,9 @@
       <c r="L91" s="5"/>
       <c r="M91" s="17"/>
       <c r="N91" s="5"/>
-      <c r="O91" s="5"/>
+      <c r="O91" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="92" spans="1:15">
       <c r="A92" s="14" t="s">
@@ -9098,7 +9100,9 @@
         <v>536</v>
       </c>
       <c r="N92" s="5"/>
-      <c r="O92" s="5"/>
+      <c r="O92" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="93" spans="1:15">
       <c r="A93" s="14" t="s">
@@ -9134,7 +9138,9 @@
       <c r="L93" s="5"/>
       <c r="M93" s="17"/>
       <c r="N93" s="5"/>
-      <c r="O93" s="5"/>
+      <c r="O93" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="94" spans="1:15">
       <c r="A94" s="14" t="s">
@@ -9170,7 +9176,9 @@
       <c r="L94" s="5"/>
       <c r="M94" s="17"/>
       <c r="N94" s="5"/>
-      <c r="O94" s="5"/>
+      <c r="O94" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="95" spans="1:15">
       <c r="A95" s="14" t="s">
@@ -9206,7 +9214,9 @@
         <v>273</v>
       </c>
       <c r="N95" s="5"/>
-      <c r="O95" s="5"/>
+      <c r="O95" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="96" spans="1:15">
       <c r="A96" s="14" t="s">
@@ -9242,7 +9252,9 @@
       <c r="L96" s="5"/>
       <c r="M96" s="5"/>
       <c r="N96" s="5"/>
-      <c r="O96" s="5"/>
+      <c r="O96" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="97" spans="1:15">
       <c r="A97" s="14" t="s">
@@ -9278,7 +9290,9 @@
         <v>483</v>
       </c>
       <c r="N97" s="5"/>
-      <c r="O97" s="5"/>
+      <c r="O97" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="98" spans="1:15">
       <c r="A98" s="14" t="s">
@@ -9316,7 +9330,9 @@
         <v>484</v>
       </c>
       <c r="N98" s="17"/>
-      <c r="O98" s="5"/>
+      <c r="O98" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="99" spans="1:15">
       <c r="A99" s="14" t="s">
@@ -9352,7 +9368,9 @@
       <c r="L99" s="5"/>
       <c r="M99" s="18"/>
       <c r="N99" s="17"/>
-      <c r="O99" s="5"/>
+      <c r="O99" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="100" spans="1:15">
       <c r="A100" s="14" t="s">
@@ -9388,7 +9406,9 @@
       <c r="L100" s="5"/>
       <c r="M100" s="18"/>
       <c r="N100" s="17"/>
-      <c r="O100" s="5"/>
+      <c r="O100" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="101" spans="1:15">
       <c r="A101" s="14" t="s">
@@ -9424,7 +9444,9 @@
         <v>486</v>
       </c>
       <c r="N101" s="17"/>
-      <c r="O101" s="5"/>
+      <c r="O101" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="102" spans="1:15">
       <c r="A102" s="14" t="s">
@@ -9461,7 +9483,9 @@
         <v>487</v>
       </c>
       <c r="N102" s="5"/>
-      <c r="O102" s="5"/>
+      <c r="O102" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="103" spans="1:15">
       <c r="A103" s="14" t="s">
@@ -9497,7 +9521,9 @@
         <v>290</v>
       </c>
       <c r="N103" s="5"/>
-      <c r="O103" s="5"/>
+      <c r="O103" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="104" spans="1:15">
       <c r="A104" s="14" t="s">
@@ -9531,7 +9557,9 @@
       <c r="L104" s="5"/>
       <c r="M104" s="5"/>
       <c r="N104" s="5"/>
-      <c r="O104" s="5"/>
+      <c r="O104" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="105" spans="1:15">
       <c r="A105" s="14" t="s">
@@ -9567,7 +9595,9 @@
         <v>204</v>
       </c>
       <c r="N105" s="5"/>
-      <c r="O105" s="5"/>
+      <c r="O105" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="106" spans="1:15">
       <c r="A106" s="14" t="s">
@@ -9603,7 +9633,9 @@
       <c r="L106" s="5"/>
       <c r="M106" s="18"/>
       <c r="N106" s="17"/>
-      <c r="O106" s="5"/>
+      <c r="O106" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="107" spans="1:15">
       <c r="A107" s="14" t="s">
@@ -9639,7 +9671,9 @@
       <c r="L107" s="5"/>
       <c r="M107" s="17"/>
       <c r="N107" s="5"/>
-      <c r="O107" s="5"/>
+      <c r="O107" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="108" spans="1:15">
       <c r="A108" s="14" t="s">
@@ -9675,7 +9709,9 @@
         <v>299</v>
       </c>
       <c r="N108" s="5"/>
-      <c r="O108" s="5"/>
+      <c r="O108" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="109" spans="1:15">
       <c r="A109" s="14" t="s">
@@ -9709,7 +9745,9 @@
       <c r="L109" s="5"/>
       <c r="M109" s="5"/>
       <c r="N109" s="5"/>
-      <c r="O109" s="5"/>
+      <c r="O109" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="110" spans="1:15">
       <c r="A110" s="14" t="s">
@@ -9745,7 +9783,9 @@
         <v>204</v>
       </c>
       <c r="N110" s="5"/>
-      <c r="O110" s="5"/>
+      <c r="O110" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="111" spans="1:15">
       <c r="A111" s="14" t="s">
@@ -9781,7 +9821,9 @@
       <c r="L111" s="5"/>
       <c r="M111" s="17"/>
       <c r="N111" s="5"/>
-      <c r="O111" s="5"/>
+      <c r="O111" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="112" spans="1:15">
       <c r="A112" s="14" t="s">
@@ -9817,7 +9859,9 @@
       <c r="L112" s="5"/>
       <c r="M112" s="17"/>
       <c r="N112" s="5"/>
-      <c r="O112" s="5"/>
+      <c r="O112" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="113" spans="1:15">
       <c r="A113" s="14" t="s">
@@ -9853,9 +9897,11 @@
         <v>509</v>
       </c>
       <c r="N113" s="5"/>
-      <c r="O113" s="5"/>
-    </row>
-    <row ht="27" r="114" spans="1:15">
+      <c r="O113" s="5" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15" ht="27">
       <c r="A114" s="14" t="s">
         <v>530</v>
       </c>
@@ -9895,7 +9941,9 @@
         <v>325</v>
       </c>
       <c r="N114" s="17"/>
-      <c r="O114" s="5"/>
+      <c r="O114" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="115" spans="1:15">
       <c r="A115" s="14" t="s">
@@ -9929,7 +9977,9 @@
       <c r="L115" s="5"/>
       <c r="M115" s="5"/>
       <c r="N115" s="5"/>
-      <c r="O115" s="5"/>
+      <c r="O115" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="116" spans="1:15">
       <c r="A116" s="14" t="s">
@@ -9965,7 +10015,9 @@
       <c r="L116" s="5"/>
       <c r="M116" s="5"/>
       <c r="N116" s="5"/>
-      <c r="O116" s="5"/>
+      <c r="O116" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="117" spans="1:15">
       <c r="A117" s="14" t="s">
@@ -10001,9 +10053,11 @@
       <c r="L117" s="5"/>
       <c r="M117" s="18"/>
       <c r="N117" s="17"/>
-      <c r="O117" s="5"/>
-    </row>
-    <row ht="27" r="118" spans="1:15">
+      <c r="O117" s="5" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15" ht="27">
       <c r="A118" s="14" t="s">
         <v>530</v>
       </c>
@@ -10039,7 +10093,9 @@
         <v>331</v>
       </c>
       <c r="N118" s="17"/>
-      <c r="O118" s="5"/>
+      <c r="O118" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="119" spans="1:15">
       <c r="A119" s="14" t="s">
@@ -10073,7 +10129,9 @@
       <c r="L119" s="5"/>
       <c r="M119" s="18"/>
       <c r="N119" s="5"/>
-      <c r="O119" s="5"/>
+      <c r="O119" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="120" spans="1:15">
       <c r="A120" s="14" t="s">
@@ -10109,11 +10167,13 @@
         <v>176</v>
       </c>
       <c r="N120" s="5"/>
-      <c r="O120" s="5"/>
+      <c r="O120" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="121" spans="1:15">
       <c r="A121" s="14" t="s">
-        <v>530</v>
+        <v>505</v>
       </c>
       <c r="B121" s="5" t="s">
         <v>315</v>
@@ -10127,23 +10187,23 @@
       <c r="E121" s="17" t="s">
         <v>306</v>
       </c>
-      <c r="F121" s="18" t="s">
-        <v>335</v>
+      <c r="F121" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="G121" s="15" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H121" s="16" t="str">
         <f>VLOOKUP(G121,KeyWords!A:B,2,FALSE)</f>
-        <v>buttonClick</v>
-      </c>
-      <c r="I121" s="5"/>
+        <v>sleep</v>
+      </c>
+      <c r="I121" s="22" t="s">
+        <v>499</v>
+      </c>
       <c r="J121" s="5"/>
       <c r="K121" s="5"/>
       <c r="L121" s="5"/>
-      <c r="M121" s="18" t="s">
-        <v>336</v>
-      </c>
+      <c r="M121" s="5"/>
       <c r="N121" s="5"/>
       <c r="O121" s="5"/>
     </row>
@@ -10163,23 +10223,23 @@
       <c r="E122" s="17" t="s">
         <v>306</v>
       </c>
-      <c r="F122" s="5" t="s">
-        <v>35</v>
+      <c r="F122" s="18" t="s">
+        <v>335</v>
       </c>
       <c r="G122" s="15" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H122" s="16" t="str">
         <f>VLOOKUP(G122,KeyWords!A:B,2,FALSE)</f>
-        <v>sleep</v>
-      </c>
-      <c r="I122" s="22" t="s">
-        <v>532</v>
-      </c>
+        <v>buttonClick</v>
+      </c>
+      <c r="I122" s="5"/>
       <c r="J122" s="5"/>
       <c r="K122" s="5"/>
       <c r="L122" s="5"/>
-      <c r="M122" s="5"/>
+      <c r="M122" s="18" t="s">
+        <v>336</v>
+      </c>
       <c r="N122" s="5"/>
       <c r="O122" s="5"/>
     </row>
@@ -10197,29 +10257,29 @@
         <v>105</v>
       </c>
       <c r="E123" s="17" t="s">
-        <v>339</v>
-      </c>
-      <c r="F123" s="18" t="s">
-        <v>142</v>
+        <v>306</v>
+      </c>
+      <c r="F123" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="G123" s="15" t="s">
-        <v>142</v>
+        <v>35</v>
       </c>
       <c r="H123" s="16" t="str">
         <f>VLOOKUP(G123,KeyWords!A:B,2,FALSE)</f>
-        <v>intoIframe</v>
-      </c>
-      <c r="I123" s="23" t="s">
-        <v>143</v>
+        <v>sleep</v>
+      </c>
+      <c r="I123" s="22" t="s">
+        <v>532</v>
       </c>
       <c r="J123" s="5"/>
       <c r="K123" s="5"/>
       <c r="L123" s="5"/>
-      <c r="M123" s="17"/>
+      <c r="M123" s="5"/>
       <c r="N123" s="5"/>
       <c r="O123" s="5"/>
     </row>
-    <row ht="27" r="124" spans="1:15">
+    <row r="124" spans="1:15">
       <c r="A124" s="14" t="s">
         <v>530</v>
       </c>
@@ -10236,32 +10296,26 @@
         <v>339</v>
       </c>
       <c r="F124" s="18" t="s">
-        <v>340</v>
+        <v>142</v>
       </c>
       <c r="G124" s="15" t="s">
-        <v>322</v>
+        <v>142</v>
       </c>
       <c r="H124" s="16" t="str">
         <f>VLOOKUP(G124,KeyWords!A:B,2,FALSE)</f>
-        <v>itemIdMultipleExpressionClick</v>
+        <v>intoIframe</v>
       </c>
       <c r="I124" s="23" t="s">
-        <v>323</v>
-      </c>
-      <c r="J124" s="23" t="s">
-        <v>324</v>
-      </c>
-      <c r="K124" s="25" t="s">
-        <v>52</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="J124" s="5"/>
+      <c r="K124" s="5"/>
       <c r="L124" s="5"/>
-      <c r="M124" s="18" t="s">
-        <v>341</v>
-      </c>
-      <c r="N124" s="17"/>
+      <c r="M124" s="17"/>
+      <c r="N124" s="5"/>
       <c r="O124" s="5"/>
     </row>
-    <row r="125" spans="1:15">
+    <row r="125" spans="1:15" ht="27">
       <c r="A125" s="14" t="s">
         <v>530</v>
       </c>
@@ -10278,21 +10332,29 @@
         <v>339</v>
       </c>
       <c r="F125" s="18" t="s">
-        <v>152</v>
+        <v>340</v>
       </c>
       <c r="G125" s="15" t="s">
-        <v>152</v>
+        <v>322</v>
       </c>
       <c r="H125" s="16" t="str">
         <f>VLOOKUP(G125,KeyWords!A:B,2,FALSE)</f>
-        <v>outIframe</v>
-      </c>
-      <c r="I125" s="5"/>
-      <c r="J125" s="5"/>
-      <c r="K125" s="5"/>
+        <v>itemIdMultipleExpressionClick</v>
+      </c>
+      <c r="I125" s="23" t="s">
+        <v>323</v>
+      </c>
+      <c r="J125" s="23" t="s">
+        <v>324</v>
+      </c>
+      <c r="K125" s="25" t="s">
+        <v>52</v>
+      </c>
       <c r="L125" s="5"/>
-      <c r="M125" s="5"/>
-      <c r="N125" s="5"/>
+      <c r="M125" s="18" t="s">
+        <v>341</v>
+      </c>
+      <c r="N125" s="17"/>
       <c r="O125" s="5"/>
     </row>
     <row r="126" spans="1:15">
@@ -10312,18 +10374,16 @@
         <v>339</v>
       </c>
       <c r="F126" s="18" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="G126" s="15" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="H126" s="16" t="str">
         <f>VLOOKUP(G126,KeyWords!A:B,2,FALSE)</f>
-        <v>intoIframe</v>
-      </c>
-      <c r="I126" s="17" t="s">
-        <v>343</v>
-      </c>
+        <v>outIframe</v>
+      </c>
+      <c r="I126" s="5"/>
       <c r="J126" s="5"/>
       <c r="K126" s="5"/>
       <c r="L126" s="5"/>
@@ -10347,22 +10407,23 @@
       <c r="E127" s="17" t="s">
         <v>339</v>
       </c>
-      <c r="F127" s="19" t="s">
-        <v>510</v>
+      <c r="F127" s="18" t="s">
+        <v>142</v>
       </c>
       <c r="G127" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="H127" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="I127" s="17"/>
+        <v>142</v>
+      </c>
+      <c r="H127" s="16" t="str">
+        <f>VLOOKUP(G127,KeyWords!A:B,2,FALSE)</f>
+        <v>intoIframe</v>
+      </c>
+      <c r="I127" s="17" t="s">
+        <v>343</v>
+      </c>
       <c r="J127" s="5"/>
       <c r="K127" s="5"/>
       <c r="L127" s="5"/>
-      <c r="M127" s="18" t="s">
-        <v>346</v>
-      </c>
+      <c r="M127" s="5"/>
       <c r="N127" s="5"/>
       <c r="O127" s="5"/>
     </row>
@@ -10382,19 +10443,16 @@
       <c r="E128" s="17" t="s">
         <v>339</v>
       </c>
-      <c r="F128" s="18" t="s">
-        <v>345</v>
+      <c r="F128" s="19" t="s">
+        <v>510</v>
       </c>
       <c r="G128" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="H128" s="16" t="str">
-        <f>VLOOKUP(G128,KeyWords!A:B,2,FALSE)</f>
-        <v>inputText</v>
-      </c>
-      <c r="I128" s="23" t="s">
-        <v>92</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="H128" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="I128" s="17"/>
       <c r="J128" s="5"/>
       <c r="K128" s="5"/>
       <c r="L128" s="5"/>
@@ -10421,21 +10479,23 @@
         <v>339</v>
       </c>
       <c r="F129" s="18" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="G129" s="15" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H129" s="16" t="str">
         <f>VLOOKUP(G129,KeyWords!A:B,2,FALSE)</f>
-        <v>buttonClick</v>
-      </c>
-      <c r="I129" s="5"/>
+        <v>inputText</v>
+      </c>
+      <c r="I129" s="23" t="s">
+        <v>92</v>
+      </c>
       <c r="J129" s="5"/>
       <c r="K129" s="5"/>
       <c r="L129" s="5"/>
       <c r="M129" s="18" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="N129" s="5"/>
       <c r="O129" s="5"/>
@@ -10457,22 +10517,22 @@
         <v>339</v>
       </c>
       <c r="F130" s="18" t="s">
-        <v>142</v>
+        <v>348</v>
       </c>
       <c r="G130" s="15" t="s">
-        <v>142</v>
+        <v>38</v>
       </c>
       <c r="H130" s="16" t="str">
         <f>VLOOKUP(G130,KeyWords!A:B,2,FALSE)</f>
-        <v>intoIframe</v>
-      </c>
-      <c r="I130" s="20" t="s">
-        <v>515</v>
-      </c>
+        <v>buttonClick</v>
+      </c>
+      <c r="I130" s="5"/>
       <c r="J130" s="5"/>
       <c r="K130" s="5"/>
       <c r="L130" s="5"/>
-      <c r="M130" s="18"/>
+      <c r="M130" s="18" t="s">
+        <v>349</v>
+      </c>
       <c r="N130" s="5"/>
       <c r="O130" s="5"/>
     </row>
@@ -10493,24 +10553,22 @@
         <v>339</v>
       </c>
       <c r="F131" s="18" t="s">
-        <v>351</v>
+        <v>142</v>
       </c>
       <c r="G131" s="15" t="s">
-        <v>51</v>
+        <v>142</v>
       </c>
       <c r="H131" s="16" t="str">
         <f>VLOOKUP(G131,KeyWords!A:B,2,FALSE)</f>
-        <v>inputText</v>
-      </c>
-      <c r="I131" s="23" t="s">
-        <v>514</v>
+        <v>intoIframe</v>
+      </c>
+      <c r="I131" s="20" t="s">
+        <v>515</v>
       </c>
       <c r="J131" s="5"/>
       <c r="K131" s="5"/>
       <c r="L131" s="5"/>
-      <c r="M131" s="18" t="s">
-        <v>352</v>
-      </c>
+      <c r="M131" s="18"/>
       <c r="N131" s="5"/>
       <c r="O131" s="5"/>
     </row>
@@ -10530,22 +10588,24 @@
       <c r="E132" s="17" t="s">
         <v>339</v>
       </c>
-      <c r="F132" s="19" t="s">
-        <v>516</v>
+      <c r="F132" s="18" t="s">
+        <v>351</v>
       </c>
       <c r="G132" s="15" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="H132" s="16" t="str">
         <f>VLOOKUP(G132,KeyWords!A:B,2,FALSE)</f>
-        <v>buttonClick</v>
-      </c>
-      <c r="I132" s="23"/>
+        <v>inputText</v>
+      </c>
+      <c r="I132" s="23" t="s">
+        <v>514</v>
+      </c>
       <c r="J132" s="5"/>
       <c r="K132" s="5"/>
       <c r="L132" s="5"/>
-      <c r="M132" s="19" t="s">
-        <v>517</v>
+      <c r="M132" s="18" t="s">
+        <v>352</v>
       </c>
       <c r="N132" s="5"/>
       <c r="O132" s="5"/>
@@ -10566,23 +10626,23 @@
       <c r="E133" s="17" t="s">
         <v>339</v>
       </c>
-      <c r="F133" s="5" t="s">
-        <v>35</v>
+      <c r="F133" s="19" t="s">
+        <v>516</v>
       </c>
       <c r="G133" s="15" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H133" s="16" t="str">
         <f>VLOOKUP(G133,KeyWords!A:B,2,FALSE)</f>
-        <v>sleep</v>
-      </c>
-      <c r="I133" s="22" t="s">
-        <v>532</v>
-      </c>
+        <v>buttonClick</v>
+      </c>
+      <c r="I133" s="23"/>
       <c r="J133" s="5"/>
       <c r="K133" s="5"/>
       <c r="L133" s="5"/>
-      <c r="M133" s="5"/>
+      <c r="M133" s="19" t="s">
+        <v>517</v>
+      </c>
       <c r="N133" s="5"/>
       <c r="O133" s="5"/>
     </row>
@@ -10602,17 +10662,19 @@
       <c r="E134" s="17" t="s">
         <v>339</v>
       </c>
-      <c r="F134" s="18" t="s">
-        <v>152</v>
+      <c r="F134" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="G134" s="15" t="s">
-        <v>152</v>
+        <v>35</v>
       </c>
       <c r="H134" s="16" t="str">
         <f>VLOOKUP(G134,KeyWords!A:B,2,FALSE)</f>
-        <v>outIframe</v>
-      </c>
-      <c r="I134" s="5"/>
+        <v>sleep</v>
+      </c>
+      <c r="I134" s="22" t="s">
+        <v>532</v>
+      </c>
       <c r="J134" s="5"/>
       <c r="K134" s="5"/>
       <c r="L134" s="5"/>
@@ -10637,22 +10699,20 @@
         <v>339</v>
       </c>
       <c r="F135" s="18" t="s">
-        <v>175</v>
+        <v>152</v>
       </c>
       <c r="G135" s="15" t="s">
-        <v>38</v>
+        <v>152</v>
       </c>
       <c r="H135" s="16" t="str">
         <f>VLOOKUP(G135,KeyWords!A:B,2,FALSE)</f>
-        <v>buttonClick</v>
+        <v>outIframe</v>
       </c>
       <c r="I135" s="5"/>
       <c r="J135" s="5"/>
       <c r="K135" s="5"/>
       <c r="L135" s="5"/>
-      <c r="M135" s="18" t="s">
-        <v>176</v>
-      </c>
+      <c r="M135" s="5"/>
       <c r="N135" s="5"/>
       <c r="O135" s="5"/>
     </row>
@@ -10673,7 +10733,7 @@
         <v>339</v>
       </c>
       <c r="F136" s="18" t="s">
-        <v>335</v>
+        <v>175</v>
       </c>
       <c r="G136" s="15" t="s">
         <v>38</v>
@@ -10708,23 +10768,23 @@
       <c r="E137" s="17" t="s">
         <v>339</v>
       </c>
-      <c r="F137" s="5" t="s">
-        <v>35</v>
+      <c r="F137" s="18" t="s">
+        <v>335</v>
       </c>
       <c r="G137" s="15" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H137" s="16" t="str">
         <f>VLOOKUP(G137,KeyWords!A:B,2,FALSE)</f>
-        <v>sleep</v>
-      </c>
-      <c r="I137" s="22" t="s">
-        <v>532</v>
-      </c>
+        <v>buttonClick</v>
+      </c>
+      <c r="I137" s="5"/>
       <c r="J137" s="5"/>
       <c r="K137" s="5"/>
       <c r="L137" s="5"/>
-      <c r="M137" s="5"/>
+      <c r="M137" s="18" t="s">
+        <v>176</v>
+      </c>
       <c r="N137" s="5"/>
       <c r="O137" s="5"/>
     </row>
@@ -10744,18 +10804,18 @@
       <c r="E138" s="17" t="s">
         <v>339</v>
       </c>
-      <c r="F138" s="18" t="s">
-        <v>142</v>
+      <c r="F138" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="G138" s="15" t="s">
-        <v>142</v>
+        <v>35</v>
       </c>
       <c r="H138" s="16" t="str">
         <f>VLOOKUP(G138,KeyWords!A:B,2,FALSE)</f>
-        <v>intoIframe</v>
-      </c>
-      <c r="I138" s="17" t="s">
-        <v>143</v>
+        <v>sleep</v>
+      </c>
+      <c r="I138" s="22" t="s">
+        <v>532</v>
       </c>
       <c r="J138" s="5"/>
       <c r="K138" s="5"/>
@@ -10781,22 +10841,22 @@
         <v>339</v>
       </c>
       <c r="F139" s="18" t="s">
-        <v>358</v>
+        <v>142</v>
       </c>
       <c r="G139" s="15" t="s">
-        <v>38</v>
+        <v>142</v>
       </c>
       <c r="H139" s="16" t="str">
         <f>VLOOKUP(G139,KeyWords!A:B,2,FALSE)</f>
-        <v>buttonClick</v>
-      </c>
-      <c r="I139" s="5"/>
+        <v>intoIframe</v>
+      </c>
+      <c r="I139" s="17" t="s">
+        <v>143</v>
+      </c>
       <c r="J139" s="5"/>
       <c r="K139" s="5"/>
       <c r="L139" s="5"/>
-      <c r="M139" s="17" t="s">
-        <v>359</v>
-      </c>
+      <c r="M139" s="5"/>
       <c r="N139" s="5"/>
       <c r="O139" s="5"/>
     </row>
@@ -10817,23 +10877,21 @@
         <v>339</v>
       </c>
       <c r="F140" s="18" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G140" s="15" t="s">
-        <v>361</v>
+        <v>38</v>
       </c>
       <c r="H140" s="16" t="str">
         <f>VLOOKUP(G140,KeyWords!A:B,2,FALSE)</f>
-        <v>assertString</v>
-      </c>
-      <c r="I140" s="17" t="s">
-        <v>362</v>
-      </c>
+        <v>buttonClick</v>
+      </c>
+      <c r="I140" s="5"/>
       <c r="J140" s="5"/>
       <c r="K140" s="5"/>
       <c r="L140" s="5"/>
       <c r="M140" s="17" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="N140" s="5"/>
       <c r="O140" s="5"/>
@@ -10848,29 +10906,31 @@
       <c r="C141" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D141" s="17" t="s">
+      <c r="D141" s="5" t="s">
         <v>105</v>
       </c>
       <c r="E141" s="17" t="s">
-        <v>364</v>
+        <v>339</v>
       </c>
       <c r="F141" s="18" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="G141" s="15" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="H141" s="16" t="str">
         <f>VLOOKUP(G141,KeyWords!A:B,2,FALSE)</f>
-        <v>closeBrowser</v>
+        <v>assertString</v>
       </c>
       <c r="I141" s="17" t="s">
-        <v>108</v>
+        <v>362</v>
       </c>
       <c r="J141" s="5"/>
       <c r="K141" s="5"/>
       <c r="L141" s="5"/>
-      <c r="M141" s="17"/>
+      <c r="M141" s="17" t="s">
+        <v>363</v>
+      </c>
       <c r="N141" s="5"/>
       <c r="O141" s="5"/>
     </row>
@@ -10882,33 +10942,33 @@
         <v>357</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>29</v>
+        <v>104</v>
       </c>
       <c r="D142" s="17" t="s">
-        <v>30</v>
+        <v>105</v>
       </c>
       <c r="E142" s="17" t="s">
         <v>364</v>
       </c>
       <c r="F142" s="18" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="G142" s="15" t="s">
-        <v>519</v>
+        <v>364</v>
       </c>
       <c r="H142" s="16" t="str">
         <f>VLOOKUP(G142,KeyWords!A:B,2,FALSE)</f>
-        <v>closeApp</v>
-      </c>
-      <c r="I142" s="24"/>
+        <v>closeBrowser</v>
+      </c>
+      <c r="I142" s="17" t="s">
+        <v>108</v>
+      </c>
       <c r="J142" s="5"/>
       <c r="K142" s="5"/>
       <c r="L142" s="5"/>
       <c r="M142" s="17"/>
       <c r="N142" s="5"/>
-      <c r="O142" s="5" t="s">
-        <v>478</v>
-      </c>
+      <c r="O142" s="5"/>
     </row>
     <row r="143" spans="1:15">
       <c r="A143" s="14" t="s">
@@ -10921,13 +10981,13 @@
         <v>29</v>
       </c>
       <c r="D143" s="17" t="s">
-        <v>215</v>
+        <v>30</v>
       </c>
       <c r="E143" s="17" t="s">
         <v>364</v>
       </c>
       <c r="F143" s="18" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G143" s="15" t="s">
         <v>519</v>
@@ -10941,37 +11001,73 @@
       <c r="K143" s="5"/>
       <c r="L143" s="5"/>
       <c r="M143" s="17"/>
-      <c r="N143" s="17"/>
+      <c r="N143" s="5"/>
       <c r="O143" s="5" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="144" spans="1:15">
+      <c r="A144" s="14" t="s">
+        <v>530</v>
+      </c>
+      <c r="B144" s="5" t="s">
+        <v>542</v>
+      </c>
+      <c r="C144" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D144" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="E144" s="17" t="s">
+        <v>364</v>
+      </c>
+      <c r="F144" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="G144" s="15" t="s">
+        <v>519</v>
+      </c>
+      <c r="H144" s="16" t="str">
+        <f>VLOOKUP(G144,KeyWords!A:B,2,FALSE)</f>
+        <v>closeApp</v>
+      </c>
+      <c r="I144" s="24"/>
+      <c r="J144" s="5"/>
+      <c r="K144" s="5"/>
+      <c r="L144" s="5"/>
+      <c r="M144" s="17"/>
+      <c r="N144" s="17"/>
+      <c r="O144" s="5" t="s">
         <v>478</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="G2:G143" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G144">
       <formula1>"浏览器,打开,打开app,关闭,关闭app,关闭窗口,切换至窗口再关闭,切换窗口,系统提示,断言,切入iframe,切入含工单id的iframe,切出iframe,等待,输入,清空,滑动至元素再单击,输入工单id,单击,双击,javaScript单击,单击含参数,根据工单id多表达式单击,根据竞价单id多表达式单击,根据托运单id多表达式单击,根据工单id单击,根据竞价单id单击,根据托运单id单击,滑动,使用index选择下拉框数据,使用value属性选择下拉框数据,使用文本选择下拉数据"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C2:C143" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C144">
       <formula1>"web,app"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="D2:D143" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D144">
       <formula1>"货主,货运站,车主,小二,水泥电商"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="I28"/>
-    <hyperlink r:id="rId2" ref="I31"/>
+    <hyperlink ref="I28" r:id="rId1"/>
+    <hyperlink ref="I31" r:id="rId2"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.69930555555555596" right="0.69930555555555596" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
   <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
-  <dimension ref="A1:P118"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
@@ -10979,18 +11075,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="12.375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="13.125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="7.5" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="24.375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="16.5" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="31.875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="24.375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="20.25" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" hidden="true" width="9.0" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="17.625" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="17.25" collapsed="true"/>
+    <col min="1" max="1" width="12.375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="7.5" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.5" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="31.875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="24.375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="20.25" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="9" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="22" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="17.625" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="17.25" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -14582,31 +14678,31 @@
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C2:C118" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C118">
       <formula1>"web,app"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="D2:D118" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D118">
       <formula1>"货主,货运站,车主,小二,水泥电商"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="G2:G118" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G118">
       <formula1>"浏览器,打开,打开app,关闭,切换窗口,系统提示,断言,切入iframe,切入含工单id的iframe,切出iframe,等待,输入,清空,滑动至元素再单击,输入工单id,单击,双击,javaScript单击,单击含参数,根据工单id多表达式单击,根据竞价单id多表达式单击,根据托运单id多表达式单击,根据工单id单击,根据竞价单id单击,根据托运单id单击,滑动,使用index选择下拉框数据,使用value属性选择下拉框数据,使用文本选择下拉数据"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="I20"/>
-    <hyperlink r:id="rId2" ref="I23"/>
-    <hyperlink r:id="rId3" ref="I3"/>
-    <hyperlink r:id="rId4" ref="I6"/>
+    <hyperlink ref="I20" r:id="rId1"/>
+    <hyperlink ref="I23" r:id="rId2"/>
+    <hyperlink ref="I3" r:id="rId3"/>
+    <hyperlink ref="I6" r:id="rId4"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.69930555555555596" right="0.69930555555555596" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <legacyDrawing r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
-  <dimension ref="A1:C33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
@@ -14614,8 +14710,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="25.875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.125" collapsed="true"/>
+    <col min="1" max="1" width="25.875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -14881,14 +14977,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.69930555555555596" right="0.69930555555555596" top="0.75"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
-  <dimension ref="A1:P12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
@@ -14915,7 +15011,7 @@
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
     </row>
-    <row ht="27" r="2" spans="1:15">
+    <row r="2" spans="1:15" ht="27">
       <c r="A2" s="14" t="s">
         <v>505</v>
       </c>
@@ -14953,7 +15049,7 @@
         <v>478</v>
       </c>
     </row>
-    <row ht="27" r="3" spans="1:15">
+    <row r="3" spans="1:15" ht="27">
       <c r="A3" s="14" t="s">
         <v>505</v>
       </c>
@@ -15027,7 +15123,7 @@
         <v>478</v>
       </c>
     </row>
-    <row ht="27" r="5" spans="1:15">
+    <row r="5" spans="1:15" ht="27">
       <c r="A5" s="14" t="s">
         <v>505</v>
       </c>
@@ -15065,7 +15161,7 @@
         <v>478</v>
       </c>
     </row>
-    <row ht="27" r="6" spans="1:15">
+    <row r="6" spans="1:15" ht="27">
       <c r="A6" s="14" t="s">
         <v>505</v>
       </c>
@@ -15141,7 +15237,7 @@
         <v>478</v>
       </c>
     </row>
-    <row ht="27" r="8" spans="1:15">
+    <row r="8" spans="1:15" ht="27">
       <c r="A8" s="14" t="s">
         <v>505</v>
       </c>
@@ -15219,7 +15315,7 @@
         <v>478</v>
       </c>
     </row>
-    <row ht="27" r="10" spans="1:15">
+    <row r="10" spans="1:15" ht="27">
       <c r="A10" s="14" t="s">
         <v>505</v>
       </c>
@@ -15295,7 +15391,7 @@
         <v>478</v>
       </c>
     </row>
-    <row ht="27" r="12" spans="1:15">
+    <row r="12" spans="1:15" ht="27">
       <c r="A12" s="14" t="s">
         <v>505</v>
       </c>
@@ -15336,18 +15432,18 @@
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="D1:D12" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D12">
       <formula1>"货主,货运站,车主,小二,水泥电商"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C1:C12" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C12">
       <formula1>"web,app"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="G1:G12" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G12">
       <formula1>"浏览器,打开,打开app,关闭,关闭窗口,切换窗口,系统提示,断言,切入iframe,切入含工单id的iframe,切出iframe,等待,输入,清空,滑动至元素再单击,输入工单id,单击,双击,javaScript单击,单击含参数,根据工单id多表达式单击,根据竞价单id多表达式单击,根据托运单id多表达式单击,根据工单id单击,根据竞价单id单击,根据托运单id单击,滑动,使用index选择下拉框数据,使用value属性选择下拉框数据,使用文本选择下拉数据"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
the seventh time commit
</commit_message>
<xml_diff>
--- a/excel_testcase/testdata.xlsx
+++ b/excel_testcase/testdata.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\UiAutomation\WuLiuUiAutomation\excel_testcase\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="7950" activeTab="1"/>
+    <workbookView activeTab="1" windowHeight="7950" windowWidth="20385" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Suite" sheetId="1" r:id="rId1"/>
-    <sheet name="HuoZhuSteps" sheetId="4" r:id="rId2"/>
-    <sheet name="GouShuiNiStep" sheetId="2" r:id="rId3"/>
-    <sheet name="KeyWords" sheetId="3" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
+    <sheet name="Suite" r:id="rId1" sheetId="1"/>
+    <sheet name="HuoZhuSteps" r:id="rId2" sheetId="4"/>
+    <sheet name="GouShuiNiStep" r:id="rId3" sheetId="2"/>
+    <sheet name="KeyWords" r:id="rId4" sheetId="3"/>
+    <sheet name="Sheet1" r:id="rId5" sheetId="5"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -30,7 +30,7 @@
     <author>作者</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment authorId="0" ref="A1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -54,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment authorId="0" ref="B1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -78,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment authorId="0" ref="C1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -102,7 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment authorId="0" ref="D1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -126,7 +126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment authorId="0" ref="E1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -150,7 +150,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment authorId="0" ref="F1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -174,7 +174,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment authorId="0" ref="G1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -198,7 +198,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment authorId="0" ref="H1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -222,7 +222,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment authorId="0" ref="M1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -246,7 +246,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment authorId="0" ref="N1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -270,7 +270,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
+    <comment authorId="0" ref="O1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -294,7 +294,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="1" shapeId="0">
+    <comment authorId="1" ref="D2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -318,7 +318,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G2" authorId="1" shapeId="0">
+    <comment authorId="1" ref="G2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -344,7 +344,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="1" shapeId="0">
+    <comment authorId="1" ref="D3" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -368,7 +368,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="1" shapeId="0">
+    <comment authorId="1" ref="I5" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -392,7 +392,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I6" authorId="1" shapeId="0">
+    <comment authorId="1" ref="I6" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -416,7 +416,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I27" authorId="1" shapeId="0">
+    <comment authorId="1" ref="I27" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -440,7 +440,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J27" authorId="2" shapeId="0">
+    <comment authorId="2" ref="J27" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -464,7 +464,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G37" authorId="1" shapeId="0">
+    <comment authorId="1" ref="G37" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -488,7 +488,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G40" authorId="1" shapeId="0">
+    <comment authorId="1" ref="G40" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -512,7 +512,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K40" authorId="1" shapeId="0">
+    <comment authorId="1" ref="K40" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -536,7 +536,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J42" authorId="1" shapeId="0">
+    <comment authorId="1" ref="J42" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -560,7 +560,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I44" authorId="1" shapeId="0">
+    <comment authorId="1" ref="I44" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -584,7 +584,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G59" authorId="1" shapeId="0">
+    <comment authorId="1" ref="G59" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -608,7 +608,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I59" authorId="1" shapeId="0">
+    <comment authorId="1" ref="I59" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -632,7 +632,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K59" authorId="1" shapeId="0">
+    <comment authorId="1" ref="K59" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -656,7 +656,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G60" authorId="1" shapeId="0">
+    <comment authorId="1" ref="G60" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -680,7 +680,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I60" authorId="1" shapeId="0">
+    <comment authorId="1" ref="I60" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -704,7 +704,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G64" authorId="1" shapeId="0">
+    <comment authorId="1" ref="G64" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -728,7 +728,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I64" authorId="1" shapeId="0">
+    <comment authorId="1" ref="I64" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -752,7 +752,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I71" authorId="1" shapeId="0">
+    <comment authorId="1" ref="I71" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -778,7 +778,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I78" authorId="1" shapeId="0">
+    <comment authorId="1" ref="I78" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -802,7 +802,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I87" authorId="1" shapeId="0">
+    <comment authorId="1" ref="I87" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -826,7 +826,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I91" authorId="1" shapeId="0">
+    <comment authorId="1" ref="I91" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -850,7 +850,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I93" authorId="1" shapeId="0">
+    <comment authorId="1" ref="I93" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -874,7 +874,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G98" authorId="1" shapeId="0">
+    <comment authorId="1" ref="G98" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -898,7 +898,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I98" authorId="1" shapeId="0">
+    <comment authorId="1" ref="I98" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -922,7 +922,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G99" authorId="1" shapeId="0">
+    <comment authorId="1" ref="G99" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -946,7 +946,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I99" authorId="1" shapeId="0">
+    <comment authorId="1" ref="I99" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -970,7 +970,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I102" authorId="1" shapeId="0">
+    <comment authorId="1" ref="I102" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -994,7 +994,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G114" authorId="1" shapeId="0">
+    <comment authorId="1" ref="G114" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1018,7 +1018,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I114" authorId="1" shapeId="0">
+    <comment authorId="1" ref="I114" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1042,7 +1042,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K114" authorId="1" shapeId="0">
+    <comment authorId="1" ref="K114" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1066,7 +1066,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G125" authorId="1" shapeId="0">
+    <comment authorId="1" ref="G125" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1090,7 +1090,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I125" authorId="1" shapeId="0">
+    <comment authorId="1" ref="I125" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1114,7 +1114,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K125" authorId="1" shapeId="0">
+    <comment authorId="1" ref="K125" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1138,7 +1138,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I132" authorId="1" shapeId="0">
+    <comment authorId="1" ref="I132" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1176,7 +1176,7 @@
     <author>joy</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment authorId="0" ref="A1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1200,7 +1200,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment authorId="0" ref="B1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1224,7 +1224,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment authorId="0" ref="C1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1248,7 +1248,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment authorId="0" ref="D1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1272,7 +1272,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment authorId="0" ref="E1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1296,7 +1296,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment authorId="0" ref="F1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1320,7 +1320,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment authorId="0" ref="G1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1344,7 +1344,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment authorId="0" ref="H1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1368,7 +1368,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment authorId="0" ref="M1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1392,7 +1392,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment authorId="0" ref="N1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1416,7 +1416,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
+    <comment authorId="0" ref="O1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1440,7 +1440,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I2" authorId="1" shapeId="0">
+    <comment authorId="1" ref="I2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1464,7 +1464,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J2" authorId="1" shapeId="0">
+    <comment authorId="1" ref="J2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1488,7 +1488,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I14" authorId="2" shapeId="0">
+    <comment authorId="2" ref="I14" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1512,7 +1512,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I19" authorId="2" shapeId="0">
+    <comment authorId="2" ref="I19" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1536,7 +1536,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J19" authorId="1" shapeId="0">
+    <comment authorId="1" ref="J19" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1560,7 +1560,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G30" authorId="2" shapeId="0">
+    <comment authorId="2" ref="G30" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1584,7 +1584,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G33" authorId="2" shapeId="0">
+    <comment authorId="2" ref="G33" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1608,7 +1608,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K33" authorId="2" shapeId="0">
+    <comment authorId="2" ref="K33" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1632,7 +1632,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K35" authorId="2" shapeId="0">
+    <comment authorId="2" ref="K35" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1656,7 +1656,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I37" authorId="2" shapeId="0">
+    <comment authorId="2" ref="I37" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1680,7 +1680,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G48" authorId="2" shapeId="0">
+    <comment authorId="2" ref="G48" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1704,7 +1704,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I48" authorId="2" shapeId="0">
+    <comment authorId="2" ref="I48" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1728,7 +1728,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K48" authorId="2" shapeId="0">
+    <comment authorId="2" ref="K48" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1752,7 +1752,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G50" authorId="2" shapeId="0">
+    <comment authorId="2" ref="G50" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1776,7 +1776,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I50" authorId="2" shapeId="0">
+    <comment authorId="2" ref="I50" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1800,7 +1800,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I56" authorId="2" shapeId="0">
+    <comment authorId="2" ref="I56" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1824,7 +1824,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I64" authorId="2" shapeId="0">
+    <comment authorId="2" ref="I64" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1848,7 +1848,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I65" authorId="2" shapeId="0">
+    <comment authorId="2" ref="I65" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1872,7 +1872,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I70" authorId="2" shapeId="0">
+    <comment authorId="2" ref="I70" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1896,7 +1896,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I72" authorId="2" shapeId="0">
+    <comment authorId="2" ref="I72" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1920,7 +1920,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I74" authorId="2" shapeId="0">
+    <comment authorId="2" ref="I74" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1944,7 +1944,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I76" authorId="2" shapeId="0">
+    <comment authorId="2" ref="I76" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1968,7 +1968,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I81" authorId="2" shapeId="0">
+    <comment authorId="2" ref="I81" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1992,7 +1992,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G85" authorId="2" shapeId="0">
+    <comment authorId="2" ref="G85" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2016,7 +2016,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I85" authorId="2" shapeId="0">
+    <comment authorId="2" ref="I85" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2040,7 +2040,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G87" authorId="2" shapeId="0">
+    <comment authorId="2" ref="G87" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2064,7 +2064,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I87" authorId="2" shapeId="0">
+    <comment authorId="2" ref="I87" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2088,7 +2088,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I90" authorId="2" shapeId="0">
+    <comment authorId="2" ref="I90" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2112,7 +2112,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I99" authorId="2" shapeId="0">
+    <comment authorId="2" ref="I99" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2136,7 +2136,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I102" authorId="1" shapeId="0">
+    <comment authorId="1" ref="I102" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2160,7 +2160,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J102" authorId="1" shapeId="0">
+    <comment authorId="1" ref="J102" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2194,7 +2194,7 @@
     <author>joy</author>
   </authors>
   <commentList>
-    <comment ref="B26" authorId="0" shapeId="0">
+    <comment authorId="0" ref="B26" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2228,7 +2228,7 @@
     <author>joy</author>
   </authors>
   <commentList>
-    <comment ref="I2" authorId="0" shapeId="0">
+    <comment authorId="0" ref="I2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2252,7 +2252,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G10" authorId="0" shapeId="0">
+    <comment authorId="0" ref="G10" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2276,7 +2276,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I10" authorId="0" shapeId="0">
+    <comment authorId="0" ref="I10" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2305,7 +2305,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2575" uniqueCount="543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2719" uniqueCount="544">
   <si>
     <t>测试用例</t>
   </si>
@@ -4967,11 +4967,15 @@
   <si>
     <t>test143</t>
   </si>
+  <si>
+    <t>测试用例执行成功</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="11">
     <font>
       <sz val="11"/>
@@ -5074,88 +5078,88 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="33">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" quotePrefix="1" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="8" numFmtId="49" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="8" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
+    <cellStyle builtinId="0" name="常规" xfId="0"/>
+    <cellStyle builtinId="8" name="超链接" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -5172,10 +5176,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -5210,7 +5214,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5245,7 +5249,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5333,7 +5337,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -5342,13 +5346,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -5358,7 +5362,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -5367,7 +5371,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -5376,7 +5380,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -5386,12 +5390,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -5422,7 +5426,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -5441,7 +5445,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -5453,8 +5457,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
@@ -5462,11 +5466,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="14.875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="36.75" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="36.75" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="23.625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -5514,48 +5518,48 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="D2:D3" type="list">
       <formula1>"YES,NO"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.69930555555555596" right="0.69930555555555596" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O144"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
+  <dimension ref="A1:P144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="I121" sqref="I121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="10.5" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="5" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="5.875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="6.125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.75" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18.625" style="12" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="40.75" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="19.5" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="18.5" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="8.125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="5.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="5.875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="6.125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.75" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="10.625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="12" width="18.625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="16.875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="12.125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="40.75" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="19.5" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="18.5" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="27">
+    <row ht="27" r="1" spans="1:15">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -7069,7 +7073,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="27">
+    <row ht="27" r="40" spans="1:15">
       <c r="A40" s="14" t="s">
         <v>530</v>
       </c>
@@ -7149,7 +7153,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="27">
+    <row ht="27" r="42" spans="1:15">
       <c r="A42" s="14" t="s">
         <v>530</v>
       </c>
@@ -7798,7 +7802,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="27">
+    <row ht="27" r="59" spans="1:15">
       <c r="A59" s="14" t="s">
         <v>530</v>
       </c>
@@ -9901,7 +9905,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="114" spans="1:15" ht="27">
+    <row ht="27" r="114" spans="1:15">
       <c r="A114" s="14" t="s">
         <v>530</v>
       </c>
@@ -10057,7 +10061,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="118" spans="1:15" ht="27">
+    <row ht="27" r="118" spans="1:15">
       <c r="A118" s="14" t="s">
         <v>530</v>
       </c>
@@ -10205,7 +10209,9 @@
       <c r="L121" s="5"/>
       <c r="M121" s="5"/>
       <c r="N121" s="5"/>
-      <c r="O121" s="5"/>
+      <c r="O121" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="122" spans="1:15">
       <c r="A122" s="14" t="s">
@@ -10241,7 +10247,9 @@
         <v>336</v>
       </c>
       <c r="N122" s="5"/>
-      <c r="O122" s="5"/>
+      <c r="O122" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="123" spans="1:15">
       <c r="A123" s="14" t="s">
@@ -10277,7 +10285,9 @@
       <c r="L123" s="5"/>
       <c r="M123" s="5"/>
       <c r="N123" s="5"/>
-      <c r="O123" s="5"/>
+      <c r="O123" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="124" spans="1:15">
       <c r="A124" s="14" t="s">
@@ -10313,9 +10323,11 @@
       <c r="L124" s="5"/>
       <c r="M124" s="17"/>
       <c r="N124" s="5"/>
-      <c r="O124" s="5"/>
-    </row>
-    <row r="125" spans="1:15" ht="27">
+      <c r="O124" s="5" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row ht="27" r="125" spans="1:15">
       <c r="A125" s="14" t="s">
         <v>530</v>
       </c>
@@ -10355,7 +10367,9 @@
         <v>341</v>
       </c>
       <c r="N125" s="17"/>
-      <c r="O125" s="5"/>
+      <c r="O125" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="126" spans="1:15">
       <c r="A126" s="14" t="s">
@@ -10389,7 +10403,9 @@
       <c r="L126" s="5"/>
       <c r="M126" s="5"/>
       <c r="N126" s="5"/>
-      <c r="O126" s="5"/>
+      <c r="O126" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="127" spans="1:15">
       <c r="A127" s="14" t="s">
@@ -10425,7 +10441,9 @@
       <c r="L127" s="5"/>
       <c r="M127" s="5"/>
       <c r="N127" s="5"/>
-      <c r="O127" s="5"/>
+      <c r="O127" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="128" spans="1:15">
       <c r="A128" s="14" t="s">
@@ -10460,7 +10478,9 @@
         <v>346</v>
       </c>
       <c r="N128" s="5"/>
-      <c r="O128" s="5"/>
+      <c r="O128" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="129" spans="1:15">
       <c r="A129" s="14" t="s">
@@ -10498,7 +10518,9 @@
         <v>346</v>
       </c>
       <c r="N129" s="5"/>
-      <c r="O129" s="5"/>
+      <c r="O129" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="130" spans="1:15">
       <c r="A130" s="14" t="s">
@@ -10534,7 +10556,9 @@
         <v>349</v>
       </c>
       <c r="N130" s="5"/>
-      <c r="O130" s="5"/>
+      <c r="O130" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="131" spans="1:15">
       <c r="A131" s="14" t="s">
@@ -10570,7 +10594,9 @@
       <c r="L131" s="5"/>
       <c r="M131" s="18"/>
       <c r="N131" s="5"/>
-      <c r="O131" s="5"/>
+      <c r="O131" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="132" spans="1:15">
       <c r="A132" s="14" t="s">
@@ -10608,7 +10634,9 @@
         <v>352</v>
       </c>
       <c r="N132" s="5"/>
-      <c r="O132" s="5"/>
+      <c r="O132" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="133" spans="1:15">
       <c r="A133" s="14" t="s">
@@ -10644,7 +10672,9 @@
         <v>517</v>
       </c>
       <c r="N133" s="5"/>
-      <c r="O133" s="5"/>
+      <c r="O133" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="134" spans="1:15">
       <c r="A134" s="14" t="s">
@@ -10680,7 +10710,9 @@
       <c r="L134" s="5"/>
       <c r="M134" s="5"/>
       <c r="N134" s="5"/>
-      <c r="O134" s="5"/>
+      <c r="O134" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="135" spans="1:15">
       <c r="A135" s="14" t="s">
@@ -10714,7 +10746,9 @@
       <c r="L135" s="5"/>
       <c r="M135" s="5"/>
       <c r="N135" s="5"/>
-      <c r="O135" s="5"/>
+      <c r="O135" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="136" spans="1:15">
       <c r="A136" s="14" t="s">
@@ -10750,7 +10784,9 @@
         <v>176</v>
       </c>
       <c r="N136" s="5"/>
-      <c r="O136" s="5"/>
+      <c r="O136" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="137" spans="1:15">
       <c r="A137" s="14" t="s">
@@ -10786,7 +10822,9 @@
         <v>176</v>
       </c>
       <c r="N137" s="5"/>
-      <c r="O137" s="5"/>
+      <c r="O137" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="138" spans="1:15">
       <c r="A138" s="14" t="s">
@@ -10822,7 +10860,9 @@
       <c r="L138" s="5"/>
       <c r="M138" s="5"/>
       <c r="N138" s="5"/>
-      <c r="O138" s="5"/>
+      <c r="O138" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="139" spans="1:15">
       <c r="A139" s="14" t="s">
@@ -10858,7 +10898,9 @@
       <c r="L139" s="5"/>
       <c r="M139" s="5"/>
       <c r="N139" s="5"/>
-      <c r="O139" s="5"/>
+      <c r="O139" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="140" spans="1:15">
       <c r="A140" s="14" t="s">
@@ -10894,7 +10936,9 @@
         <v>359</v>
       </c>
       <c r="N140" s="5"/>
-      <c r="O140" s="5"/>
+      <c r="O140" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="141" spans="1:15">
       <c r="A141" s="14" t="s">
@@ -10932,7 +10976,9 @@
         <v>363</v>
       </c>
       <c r="N141" s="5"/>
-      <c r="O141" s="5"/>
+      <c r="O141" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="142" spans="1:15">
       <c r="A142" s="14" t="s">
@@ -10968,7 +11014,9 @@
       <c r="L142" s="5"/>
       <c r="M142" s="17"/>
       <c r="N142" s="5"/>
-      <c r="O142" s="5"/>
+      <c r="O142" s="5" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="143" spans="1:15">
       <c r="A143" s="14" t="s">
@@ -11045,29 +11093,29 @@
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G144">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="G2:G144" type="list">
       <formula1>"浏览器,打开,打开app,关闭,关闭app,关闭窗口,切换至窗口再关闭,切换窗口,系统提示,断言,切入iframe,切入含工单id的iframe,切出iframe,等待,输入,清空,滑动至元素再单击,输入工单id,单击,双击,javaScript单击,单击含参数,根据工单id多表达式单击,根据竞价单id多表达式单击,根据托运单id多表达式单击,根据工单id单击,根据竞价单id单击,根据托运单id单击,滑动,使用index选择下拉框数据,使用value属性选择下拉框数据,使用文本选择下拉数据"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C144">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C2:C144" type="list">
       <formula1>"web,app"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D144">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="D2:D144" type="list">
       <formula1>"货主,货运站,车主,小二,水泥电商"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="I28" r:id="rId1"/>
-    <hyperlink ref="I31" r:id="rId2"/>
+    <hyperlink r:id="rId1" ref="I28"/>
+    <hyperlink r:id="rId2" ref="I31"/>
   </hyperlinks>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.69930555555555596" right="0.69930555555555596" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId3"/>
   <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O118"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
+  <dimension ref="A1:P118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
@@ -11075,18 +11123,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="12.375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="7.5" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.5" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="31.875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="24.375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="20.25" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="22" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="17.625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="17.25" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="12.375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="7.5" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="31.875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="24.375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="20.25" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" hidden="true" width="9.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="17.625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="17.25" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -14678,31 +14726,31 @@
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C118">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C2:C118" type="list">
       <formula1>"web,app"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D118">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="D2:D118" type="list">
       <formula1>"货主,货运站,车主,小二,水泥电商"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G118">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="G2:G118" type="list">
       <formula1>"浏览器,打开,打开app,关闭,切换窗口,系统提示,断言,切入iframe,切入含工单id的iframe,切出iframe,等待,输入,清空,滑动至元素再单击,输入工单id,单击,双击,javaScript单击,单击含参数,根据工单id多表达式单击,根据竞价单id多表达式单击,根据托运单id多表达式单击,根据工单id单击,根据竞价单id单击,根据托运单id单击,滑动,使用index选择下拉框数据,使用value属性选择下拉框数据,使用文本选择下拉数据"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="I20" r:id="rId1"/>
-    <hyperlink ref="I23" r:id="rId2"/>
-    <hyperlink ref="I3" r:id="rId3"/>
-    <hyperlink ref="I6" r:id="rId4"/>
+    <hyperlink r:id="rId1" ref="I20"/>
+    <hyperlink r:id="rId2" ref="I23"/>
+    <hyperlink r:id="rId3" ref="I3"/>
+    <hyperlink r:id="rId4" ref="I6"/>
   </hyperlinks>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.69930555555555596" right="0.69930555555555596" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
   <legacyDrawing r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
@@ -14710,8 +14758,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="25.875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="25.875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -14977,14 +15025,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.69930555555555596" right="0.69930555555555596" top="0.75"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
@@ -15011,7 +15059,7 @@
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
     </row>
-    <row r="2" spans="1:15" ht="27">
+    <row ht="27" r="2" spans="1:15">
       <c r="A2" s="14" t="s">
         <v>505</v>
       </c>
@@ -15049,7 +15097,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="27">
+    <row ht="27" r="3" spans="1:15">
       <c r="A3" s="14" t="s">
         <v>505</v>
       </c>
@@ -15123,7 +15171,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="27">
+    <row ht="27" r="5" spans="1:15">
       <c r="A5" s="14" t="s">
         <v>505</v>
       </c>
@@ -15161,7 +15209,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="27">
+    <row ht="27" r="6" spans="1:15">
       <c r="A6" s="14" t="s">
         <v>505</v>
       </c>
@@ -15237,7 +15285,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="27">
+    <row ht="27" r="8" spans="1:15">
       <c r="A8" s="14" t="s">
         <v>505</v>
       </c>
@@ -15315,7 +15363,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="27">
+    <row ht="27" r="10" spans="1:15">
       <c r="A10" s="14" t="s">
         <v>505</v>
       </c>
@@ -15391,7 +15439,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="27">
+    <row ht="27" r="12" spans="1:15">
       <c r="A12" s="14" t="s">
         <v>505</v>
       </c>
@@ -15432,18 +15480,18 @@
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D12">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="D1:D12" type="list">
       <formula1>"货主,货运站,车主,小二,水泥电商"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C12">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C1:C12" type="list">
       <formula1>"web,app"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G12">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="G1:G12" type="list">
       <formula1>"浏览器,打开,打开app,关闭,关闭窗口,切换窗口,系统提示,断言,切入iframe,切入含工单id的iframe,切出iframe,等待,输入,清空,滑动至元素再单击,输入工单id,单击,双击,javaScript单击,单击含参数,根据工单id多表达式单击,根据竞价单id多表达式单击,根据托运单id多表达式单击,根据工单id单击,根据竞价单id单击,根据托运单id单击,滑动,使用index选择下拉框数据,使用value属性选择下拉框数据,使用文本选择下拉数据"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
the eighth time commit
</commit_message>
<xml_diff>
--- a/excel_testcase/testdata.xlsx
+++ b/excel_testcase/testdata.xlsx
@@ -2305,7 +2305,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2719" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2954" uniqueCount="544">
   <si>
     <t>测试用例</t>
   </si>
@@ -5518,7 +5518,7 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
     </row>
   </sheetData>

</xml_diff>